<commit_message>
Insert function IDs and update class diagram
Add functions Ids to the code information column in rtm and update class diagram
</commit_message>
<xml_diff>
--- a/2-Reqs/RTM.xlsx
+++ b/2-Reqs/RTM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Foodies\2-Reqs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iti intake 43\quality assurance workshop\update by coach amr\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4466B0FF-7641-4760-BEB9-03181622420F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="traceability matrix" sheetId="5" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>status</t>
   </si>
@@ -61,9 +60,6 @@
     <t>Design.ID</t>
   </si>
   <si>
-    <t>Feature.ID</t>
-  </si>
-  <si>
     <t>TC.ID</t>
   </si>
   <si>
@@ -76,9 +72,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>FT-01</t>
-  </si>
-  <si>
     <t>TC-01</t>
   </si>
   <si>
@@ -157,9 +150,6 @@
     <t>SRS-US-11</t>
   </si>
   <si>
-    <t>Confirm order items and use my points for discount</t>
-  </si>
-  <si>
     <t xml:space="preserve">Make sure the order is submitted from the system and delivery is on his way </t>
   </si>
   <si>
@@ -227,13 +217,82 @@
   </si>
   <si>
     <t>edit account information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+F_REG_01
+F_REG_02
+F_REG_03
+F_REG_04
+F_REG_05
+F_REG_06
+</t>
+  </si>
+  <si>
+    <t>F_LOGIN_01
+F_LOGIN_02
+F_LOGIN_03</t>
+  </si>
+  <si>
+    <t>F_PASSREST_01
+F_PASSREST_02
+F_PASSREST_03
+F_PASSREST_04</t>
+  </si>
+  <si>
+    <t>Function.ID</t>
+  </si>
+  <si>
+    <t>F_Home_04</t>
+  </si>
+  <si>
+    <t>F_Home_01</t>
+  </si>
+  <si>
+    <t>F_Home_02
+F_Home_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_ACC_01
+F_ACC_02
+F_ACC_03
+</t>
+  </si>
+  <si>
+    <t>F_ACC_04
+F_ACC_05
+F_ACC_06
+F_ACC_07
+F_ACC_08</t>
+  </si>
+  <si>
+    <t>F_ADDOFF_01
+F_ADDOFF_02
+F_DELOFF_01
+F_DELOFF_02
+F_ADDREST_01
+F_ADDREST_02
+F_DELREST_01
+F_DELREST_02
+F_ADDMENU_01
+F_ADDMENU_02
+F_DELMENU_01
+F_DELMENU_02
+F_DELUSER_01
+F_DELUSER_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm order items </t>
+  </si>
+  <si>
+    <t>Deleted by the customer Mr.omar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -343,8 +402,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,20 +418,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -435,8 +488,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -699,191 +758,257 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1095,445 +1220,453 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="40"/>
+    <col min="2" max="2" width="35.6640625" style="40" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" style="40" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="40" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="40" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="29.5546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="40"/>
+    <col min="10" max="10" width="24.44140625" style="40" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="40"/>
+    <col min="12" max="12" width="23.109375" style="40" customWidth="1"/>
+    <col min="13" max="16384" width="12.5546875" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
-    <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
+    <row r="2" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
-    <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:13" ht="25.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="50" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="51" t="s">
+      <c r="I3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="48" t="s">
+      <c r="J3" s="42"/>
+      <c r="K3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="49"/>
-      <c r="N3" s="37"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>0</v>
-      </c>
+      <c r="B5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="38"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="45"/>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="45"/>
+    </row>
+    <row r="7" spans="1:13" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="45"/>
+    </row>
+    <row r="8" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="E8" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G8" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="45"/>
+    </row>
+    <row r="9" spans="1:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="45"/>
+    </row>
+    <row r="10" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="45"/>
+    </row>
+    <row r="11" spans="1:13" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="45"/>
+    </row>
+    <row r="12" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="11" t="s">
+      <c r="G12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="45"/>
+    </row>
+    <row r="13" spans="1:13" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="45"/>
+    </row>
+    <row r="14" spans="1:13" ht="201.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="1"/>
+      <c r="B14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="45"/>
     </row>
-    <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="1"/>
+    <row r="15" spans="1:13" s="70" customFormat="1" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="69"/>
     </row>
-    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="55"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="13" t="s">
+    <row r="16" spans="1:13" s="70" customFormat="1" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="63"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="G16" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" ht="46.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="1"/>
+      <c r="H16" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="68"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="17">
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
-    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A1:M2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
@@ -1542,22 +1675,19 @@
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="A8:A13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="L4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4" display="Feature.ID"/>
+    <hyperlink ref="I4" r:id="rId5"/>
+    <hyperlink ref="K4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>

</xml_diff>

<commit_message>
update rtm and class diagram
add function ids in code information column
</commit_message>
<xml_diff>
--- a/2-Reqs/RTM.xlsx
+++ b/2-Reqs/RTM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Foodies\2-Reqs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iti intake 43\quality assurance workshop\update by coach amr\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4466B0FF-7641-4760-BEB9-03181622420F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="traceability matrix" sheetId="5" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>status</t>
   </si>
@@ -61,9 +60,6 @@
     <t>Design.ID</t>
   </si>
   <si>
-    <t>Feature.ID</t>
-  </si>
-  <si>
     <t>TC.ID</t>
   </si>
   <si>
@@ -76,9 +72,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>FT-01</t>
-  </si>
-  <si>
     <t>TC-01</t>
   </si>
   <si>
@@ -157,9 +150,6 @@
     <t>SRS-US-11</t>
   </si>
   <si>
-    <t>Confirm order items and use my points for discount</t>
-  </si>
-  <si>
     <t xml:space="preserve">Make sure the order is submitted from the system and delivery is on his way </t>
   </si>
   <si>
@@ -227,13 +217,82 @@
   </si>
   <si>
     <t>edit account information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+F_REG_01
+F_REG_02
+F_REG_03
+F_REG_04
+F_REG_05
+F_REG_06
+</t>
+  </si>
+  <si>
+    <t>F_LOGIN_01
+F_LOGIN_02
+F_LOGIN_03</t>
+  </si>
+  <si>
+    <t>F_PASSREST_01
+F_PASSREST_02
+F_PASSREST_03
+F_PASSREST_04</t>
+  </si>
+  <si>
+    <t>Function.ID</t>
+  </si>
+  <si>
+    <t>F_Home_04</t>
+  </si>
+  <si>
+    <t>F_Home_01</t>
+  </si>
+  <si>
+    <t>F_Home_02
+F_Home_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_ACC_01
+F_ACC_02
+F_ACC_03
+</t>
+  </si>
+  <si>
+    <t>F_ACC_04
+F_ACC_05
+F_ACC_06
+F_ACC_07
+F_ACC_08</t>
+  </si>
+  <si>
+    <t>F_ADDOFF_01
+F_ADDOFF_02
+F_DELOFF_01
+F_DELOFF_02
+F_ADDREST_01
+F_ADDREST_02
+F_DELREST_01
+F_DELREST_02
+F_ADDMENU_01
+F_ADDMENU_02
+F_DELMENU_01
+F_DELMENU_02
+F_DELUSER_01
+F_DELUSER_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm order items </t>
+  </si>
+  <si>
+    <t>Deleted by the customer Mr.omar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -343,8 +402,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,20 +418,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -435,8 +488,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -699,191 +758,257 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1095,445 +1220,453 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="40"/>
+    <col min="2" max="2" width="35.6640625" style="40" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" style="40" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="40" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="40" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="29.5546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="40"/>
+    <col min="10" max="10" width="24.44140625" style="40" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="40"/>
+    <col min="12" max="12" width="23.109375" style="40" customWidth="1"/>
+    <col min="13" max="16384" width="12.5546875" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
-    <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
+    <row r="2" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
-    <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:13" ht="25.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="50" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="51" t="s">
+      <c r="I3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="48" t="s">
+      <c r="J3" s="42"/>
+      <c r="K3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="49"/>
-      <c r="N3" s="37"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>0</v>
-      </c>
+      <c r="B5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="38"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="45"/>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="45"/>
+    </row>
+    <row r="7" spans="1:13" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="45"/>
+    </row>
+    <row r="8" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="E8" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G8" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="45"/>
+    </row>
+    <row r="9" spans="1:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="45"/>
+    </row>
+    <row r="10" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="45"/>
+    </row>
+    <row r="11" spans="1:13" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="45"/>
+    </row>
+    <row r="12" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="11" t="s">
+      <c r="G12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="45"/>
+    </row>
+    <row r="13" spans="1:13" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="45"/>
+    </row>
+    <row r="14" spans="1:13" ht="201.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="1"/>
+      <c r="B14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="45"/>
     </row>
-    <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="1"/>
+    <row r="15" spans="1:13" s="70" customFormat="1" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="69"/>
     </row>
-    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="55"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="13" t="s">
+    <row r="16" spans="1:13" s="70" customFormat="1" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="63"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="G16" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" ht="46.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="1"/>
+      <c r="H16" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="68"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="17">
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
-    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A1:M2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
@@ -1542,22 +1675,19 @@
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="A8:A13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="L4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4" display="Feature.ID"/>
+    <hyperlink ref="I4" r:id="rId5"/>
+    <hyperlink ref="K4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>

</xml_diff>

<commit_message>
Update RTM and Test Case Report
</commit_message>
<xml_diff>
--- a/2-Reqs/RTM.xlsx
+++ b/2-Reqs/RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohip\Documents\GitHub\Foodies\2-Reqs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B046F734-838A-43F6-8B0A-AF3D7C088C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46C81EB-F869-400A-9398-78FB5616F6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="traceability matrix" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="127">
   <si>
     <t>status</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>Function.ID</t>
-  </si>
-  <si>
-    <t>F_Home_04</t>
   </si>
   <si>
     <t>F_Home_01</t>
@@ -467,6 +464,11 @@
     <t>TC-MyACC-1
 -
 TC-MyACC-12</t>
+  </si>
+  <si>
+    <t>TC-HP-13
+TC-HP-14
+TC-HP-15</t>
   </si>
 </sst>
 </file>
@@ -701,7 +703,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -881,17 +883,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -967,7 +958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -975,216 +966,240 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1193,36 +1208,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1443,650 +1428,623 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="19"/>
-    <col min="2" max="2" width="35.6640625" style="19" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="29.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="19"/>
-    <col min="11" max="11" width="23.109375" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="12.5546875" style="19"/>
+    <col min="1" max="1" width="12.5546875" style="18"/>
+    <col min="2" max="2" width="35.6640625" style="18" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="29.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="18"/>
+    <col min="11" max="11" width="23.109375" style="18" customWidth="1"/>
+    <col min="12" max="16384" width="12.5546875" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
     </row>
     <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
     </row>
     <row r="3" spans="1:12" ht="25.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="62" t="s">
+      <c r="B3" s="69"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="58" t="s">
+      <c r="E3" s="67"/>
+      <c r="F3" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="20" t="s">
+      <c r="G3" s="67"/>
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="59"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="67"/>
     </row>
     <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="73" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="22"/>
+      <c r="I5" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="75"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="66"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="22"/>
+      <c r="I6" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="1:12" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="66"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="22"/>
+      <c r="I7" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="81" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="74"/>
+      <c r="H8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:12" ht="101.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="79"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="79"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="1:12" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="79"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="85" t="s">
+      <c r="I11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="61"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="71"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="3" t="s">
+      <c r="J12" s="4"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F13" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G13" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="22"/>
-    </row>
-    <row r="11" spans="1:12" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="22"/>
-    </row>
-    <row r="12" spans="1:12" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="22"/>
-    </row>
-    <row r="13" spans="1:12" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="53"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="33"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="34"/>
+    </row>
+    <row r="14" spans="1:12" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="22"/>
-    </row>
-    <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="35"/>
-    </row>
-    <row r="15" spans="1:12" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="81" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="83" t="s">
+      <c r="F14" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="38"/>
+    </row>
+    <row r="15" spans="1:12" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="55"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="38"/>
+    </row>
+    <row r="16" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+    </row>
+    <row r="17" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+    </row>
+    <row r="18" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="I18" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+    </row>
+    <row r="20" spans="1:12" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+    </row>
+    <row r="21" spans="1:12" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+    </row>
+    <row r="22" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="52"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
-    </row>
-    <row r="16" spans="1:12" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
-      <c r="B16" s="82"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39"/>
-    </row>
-    <row r="17" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="78" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="42" t="s">
+      <c r="D22" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="I17" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-    </row>
-    <row r="18" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-    </row>
-    <row r="19" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="I19" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-    </row>
-    <row r="20" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="G20" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="I20" s="50" t="s">
+      <c r="H22" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I22" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-    </row>
-    <row r="21" spans="1:12" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-    </row>
-    <row r="22" spans="1:12" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="I22" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-    </row>
-    <row r="23" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
-      <c r="B23" s="77"/>
-      <c r="C23" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="I23" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="50"/>
     </row>
     <row r="33" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I33" s="51"/>
+      <c r="I33" s="50"/>
     </row>
     <row r="34" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I34" s="51"/>
+      <c r="I34" s="50"/>
     </row>
     <row r="35" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I35" s="51"/>
-    </row>
-    <row r="36" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I36" s="51"/>
+      <c r="I35" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="B17:B23"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="A1:L2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A3:C3"/>
@@ -2094,10 +2052,15 @@
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="C8:C12"/>
     <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>

</xml_diff>